<commit_message>
ran cadaver and tumor iarc rtx
</commit_message>
<xml_diff>
--- a/metadata_files/variant_validation.xlsx
+++ b/metadata_files/variant_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF81245-1833-5E48-9A2A-628B33E8FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E1FAB6-C035-994B-94C1-85B03AC7D1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="520" yWindow="1420" windowWidth="38400" windowHeight="19540" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -1532,12 +1532,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="1.33203125" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>

</xml_diff>

<commit_message>
started plot modifications, ran iarc tumors and cadaver
</commit_message>
<xml_diff>
--- a/metadata_files/variant_validation.xlsx
+++ b/metadata_files/variant_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdp2019/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5365C0-B4BF-A842-84DA-3B2FB421497B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33B4DB0-A1DC-BF4D-A259-266A80CF3624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15140" yWindow="500" windowWidth="23260" windowHeight="20460" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="359">
   <si>
     <t>order</t>
   </si>
@@ -812,18 +812,12 @@
     <t>F1_S1_CP2486</t>
   </si>
   <si>
-    <t>Standard has no peaks, but has two co-eluting fragments (at two different time points)</t>
-  </si>
-  <si>
     <t>1 peak sadly, not including quant</t>
   </si>
   <si>
     <t>F1_S1_CP3025</t>
   </si>
   <si>
-    <t>F3_S1_CP2212</t>
-  </si>
-  <si>
     <t>2 peaks, one quant and other not</t>
   </si>
   <si>
@@ -890,9 +884,6 @@
     <t>F1_S1_CP3021</t>
   </si>
   <si>
-    <t>maybe very small peaks on sample but there</t>
-  </si>
-  <si>
     <t>really nice co-eluting level 1 around 7.75 but not what algorithm picked</t>
   </si>
   <si>
@@ -914,9 +905,6 @@
     <t>F1_S1_CP3068</t>
   </si>
   <si>
-    <t>zoom in on y axis</t>
-  </si>
-  <si>
     <t>F3_S1_CP3193</t>
   </si>
   <si>
@@ -971,12 +959,6 @@
     <t>one giant peak, no other co-elute, other one failed too</t>
   </si>
   <si>
-    <t>removed fragment</t>
-  </si>
-  <si>
-    <t>zoom Y</t>
-  </si>
-  <si>
     <t>remove fragment?</t>
   </si>
   <si>
@@ -989,27 +971,12 @@
     <t>F1_S1_CP2225</t>
   </si>
   <si>
-    <t>eliminate to 207.0651 and 207.0651 only</t>
-  </si>
-  <si>
-    <t>zoom to individual fragments</t>
-  </si>
-  <si>
-    <t>zoom to two fragments</t>
-  </si>
-  <si>
     <t>noise</t>
   </si>
   <si>
     <t>standards good, sample sucks</t>
   </si>
   <si>
-    <t>zoom to 200.0698, expand x axis right?</t>
-  </si>
-  <si>
-    <t>zoom to individual fragments, expand x?</t>
-  </si>
-  <si>
     <t>enrmous peak</t>
   </si>
   <si>
@@ -1043,9 +1010,6 @@
     <t>F4_S2_CP2331</t>
   </si>
   <si>
-    <t>very hard to call co elution as quant peak is basically nois</t>
-  </si>
-  <si>
     <t>F2_S1_CP3174</t>
   </si>
   <si>
@@ -1064,21 +1028,12 @@
     <t>F2_S2_CP2187</t>
   </si>
   <si>
-    <t>zoom y axis, fragments</t>
-  </si>
-  <si>
     <t>Nice peak but only one</t>
   </si>
   <si>
-    <t>zoom and fragments</t>
-  </si>
-  <si>
     <t>F6_S2_CP2133</t>
   </si>
   <si>
-    <t>zoom and fragmetns</t>
-  </si>
-  <si>
     <t>1 peak that is messy, not defensible</t>
   </si>
   <si>
@@ -1103,9 +1058,6 @@
     <t>state</t>
   </si>
   <si>
-    <t>not used</t>
-  </si>
-  <si>
     <t>failed</t>
   </si>
   <si>
@@ -1116,6 +1068,54 @@
   </si>
   <si>
     <t>fragments are tiny on sample but co-elute in standard well so keeping</t>
+  </si>
+  <si>
+    <t>initial huge peak way to left but not annotated one</t>
+  </si>
+  <si>
+    <t>final (check frag)</t>
+  </si>
+  <si>
+    <t>modify</t>
+  </si>
+  <si>
+    <t>removed standard, zoomed Y axis, called level 2</t>
+  </si>
+  <si>
+    <t>very difficult to call these peaks when zooming in, Fail</t>
+  </si>
+  <si>
+    <t>F6_S1_CP2212</t>
+  </si>
+  <si>
+    <t>maybe coelution if look closely on x</t>
+  </si>
+  <si>
+    <t>very difficult to call coeluting peaks, fail</t>
+  </si>
+  <si>
+    <t>showed plot with and without major peak</t>
+  </si>
+  <si>
+    <t>maybe knock to level 2 after zoom and frag</t>
+  </si>
+  <si>
+    <t>alternate</t>
+  </si>
+  <si>
+    <t>final- modified</t>
+  </si>
+  <si>
+    <t>very hard to call this anything more than noise, failed</t>
+  </si>
+  <si>
+    <t>removed fragment (before run)</t>
+  </si>
+  <si>
+    <t>hard to call this anything other than noise; fail</t>
+  </si>
+  <si>
+    <t>Consider making level 2 but move to smaller x window</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1200,6 +1200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,7 +1539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1552,8 +1553,8 @@
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="7.1640625" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1574,22 +1575,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>236</v>
@@ -1597,2426 +1598,2394 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="H2" s="1">
-        <v>7.85</v>
+        <v>6.3</v>
       </c>
       <c r="I2" s="1">
-        <v>7.9249999999999998</v>
+        <v>6.6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>284</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>285</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1">
-        <v>13.25</v>
+        <v>4.3</v>
       </c>
       <c r="I3" s="1">
-        <v>13.45</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>128</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="5">
+        <v>129</v>
+      </c>
+      <c r="F4" s="6">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="H4" s="1">
-        <v>13.425000000000001</v>
+        <v>7.3</v>
       </c>
       <c r="I4" s="1">
-        <v>13.574999999999999</v>
+        <v>7.5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>340</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="L4" s="1" t="s">
-        <v>314</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="5">
+        <v>142</v>
+      </c>
+      <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>290</v>
+        <v>333</v>
       </c>
       <c r="H5" s="1">
-        <v>3</v>
+        <v>17.8</v>
       </c>
       <c r="I5" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K5" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>334</v>
+      </c>
       <c r="L5" s="1" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="5">
+        <v>87</v>
+      </c>
+      <c r="F6" s="6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>192</v>
+        <v>348</v>
       </c>
       <c r="H6" s="1">
-        <v>6.35</v>
+        <v>11.9</v>
       </c>
       <c r="I6" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K6" s="1"/>
+        <v>12.2</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>349</v>
+      </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="5">
+        <v>61</v>
+      </c>
+      <c r="F7" s="8">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="H7" s="1">
-        <v>6.375</v>
+        <v>19.3</v>
       </c>
       <c r="I7" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="5">
+        <v>154</v>
+      </c>
+      <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
       <c r="H8" s="1">
-        <v>9.0500000000000007</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="I8" s="1">
-        <v>9.2249999999999996</v>
-      </c>
-      <c r="J8" s="1" t="s">
+        <v>8.35</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>195</v>
+        <v>279</v>
       </c>
       <c r="H9" s="1">
-        <v>9.5749999999999993</v>
+        <v>3.8250000000000002</v>
       </c>
       <c r="I9" s="1">
-        <v>9.7750000000000004</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="5">
+        <v>148</v>
+      </c>
+      <c r="F10" s="6">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="H10" s="1">
-        <v>3.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I10" s="1">
-        <v>3.95</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>352</v>
+        <v>10.1</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>89</v>
+        <v>167</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="5">
+        <v>168</v>
+      </c>
+      <c r="F11" s="6">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>324</v>
+        <v>262</v>
       </c>
       <c r="H11" s="1">
-        <v>9.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>9.65</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>352</v>
+        <v>19.7</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>323</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="5">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="H12" s="1">
-        <v>11.2</v>
+        <v>7.9749999999999996</v>
       </c>
       <c r="I12" s="1">
-        <v>11.3575</v>
+        <v>8.15</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K12" s="1"/>
+        <v>354</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="L12" s="1" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="5">
+        <v>49</v>
+      </c>
+      <c r="F13" s="8">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>241</v>
+        <v>286</v>
       </c>
       <c r="H13" s="1">
-        <v>22.3</v>
+        <v>13.725</v>
       </c>
       <c r="I13" s="1">
-        <v>22.45</v>
+        <v>13.85</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="F14" s="5">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="H14" s="1">
-        <v>9.4499999999999993</v>
+        <v>7.85</v>
       </c>
       <c r="I14" s="1">
-        <v>9.65</v>
+        <v>7.9249999999999998</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>243</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="F15" s="5">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>327</v>
+        <v>282</v>
       </c>
       <c r="H15" s="1">
-        <v>9.35</v>
+        <v>13.25</v>
       </c>
       <c r="I15" s="1">
-        <v>9.5500000000000007</v>
+        <v>13.45</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="F16" s="5">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>247</v>
+        <v>309</v>
       </c>
       <c r="H16" s="1">
-        <v>2.25</v>
+        <v>13.425000000000001</v>
       </c>
       <c r="I16" s="1">
-        <v>2.5</v>
+        <v>13.574999999999999</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="F17" s="5">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
       <c r="H17" s="1">
-        <v>8.0250000000000004</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1">
-        <v>8.25</v>
+        <v>3.4</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="F18" s="5">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>340</v>
+        <v>192</v>
       </c>
       <c r="H18" s="1">
-        <v>18</v>
+        <v>6.35</v>
       </c>
       <c r="I18" s="1">
-        <v>18.149999999999999</v>
+        <v>6.5</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>145</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="H19" s="1">
-        <v>9.8000000000000007</v>
+        <v>6.375</v>
       </c>
       <c r="I19" s="1">
-        <v>10.102499999999999</v>
+        <v>6.5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>154</v>
+        <v>75</v>
       </c>
       <c r="F20" s="5">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>263</v>
+        <v>193</v>
       </c>
       <c r="H20" s="1">
-        <v>7.7</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="I20" s="1">
-        <v>7.875</v>
+        <v>9.2249999999999996</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>164</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="F21" s="5">
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>344</v>
+        <v>195</v>
       </c>
       <c r="H21" s="1">
-        <v>6.6</v>
+        <v>9.5749999999999993</v>
       </c>
       <c r="I21" s="1">
-        <v>6.75</v>
+        <v>9.7750000000000004</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>172</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>173</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="F22" s="5">
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>347</v>
+        <v>196</v>
       </c>
       <c r="H22" s="1">
-        <v>4.9000000000000004</v>
+        <v>3.8</v>
       </c>
       <c r="I22" s="1">
-        <v>5.05</v>
+        <v>3.95</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="H23" s="1">
-        <v>4.9000000000000004</v>
+        <v>9.4</v>
       </c>
       <c r="I23" s="1">
-        <v>5.0999999999999996</v>
+        <v>9.65</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>237</v>
+        <v>92</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>200</v>
+        <v>93</v>
       </c>
       <c r="F24" s="5">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
       <c r="H24" s="1">
-        <v>6.35</v>
+        <v>11.2</v>
       </c>
       <c r="I24" s="1">
-        <v>6.45</v>
+        <v>11.3575</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>217</v>
+        <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>218</v>
+        <v>105</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>294</v>
+        <v>241</v>
       </c>
       <c r="H25" s="1">
-        <v>6.0724999999999998</v>
+        <v>22.3</v>
       </c>
       <c r="I25" s="1">
-        <v>6.25</v>
+        <v>22.45</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="F26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="H26" s="1">
-        <v>7.4</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="I26" s="1">
-        <v>7.5250000000000004</v>
+        <v>9.65</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
-        <v>28</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F27" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="H27" s="1">
-        <v>19.45</v>
+        <v>9.35</v>
       </c>
       <c r="I27" s="1">
-        <v>19.600000000000001</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>330</v>
+        <v>247</v>
       </c>
       <c r="H28" s="1">
-        <v>4.3</v>
+        <v>2.25</v>
       </c>
       <c r="I28" s="1">
-        <v>4.45</v>
+        <v>2.5</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F29" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>332</v>
+        <v>248</v>
       </c>
       <c r="H29" s="1">
-        <v>4.25</v>
+        <v>8.0250000000000004</v>
       </c>
       <c r="I29" s="1">
-        <v>4.45</v>
+        <v>8.25</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="F30" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="H30" s="1">
-        <v>11.05</v>
+        <v>18</v>
       </c>
       <c r="I30" s="1">
-        <v>11.25</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="F31" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>350</v>
+        <v>249</v>
       </c>
       <c r="H31" s="1">
-        <v>17.149999999999999</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I31" s="1">
-        <v>17.45</v>
+        <v>10.102499999999999</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="F32" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="H32" s="1">
-        <v>7.4</v>
+        <v>7.7</v>
       </c>
       <c r="I32" s="1">
-        <v>7.55</v>
+        <v>7.875</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>221</v>
+        <v>163</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>222</v>
+        <v>165</v>
       </c>
       <c r="F33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>272</v>
+        <v>330</v>
       </c>
       <c r="H33" s="1">
-        <v>5.15</v>
+        <v>6.6</v>
       </c>
       <c r="I33" s="1">
-        <v>5.3</v>
+        <v>6.75</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
       <c r="F34" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>299</v>
+        <v>332</v>
       </c>
       <c r="H34" s="1">
-        <v>12.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I34" s="1">
-        <v>12.875</v>
+        <v>5.05</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="F35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>273</v>
+        <v>336</v>
       </c>
       <c r="H35" s="1">
-        <v>7.2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I35" s="1">
-        <v>7.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F36" s="5">
-        <v>2</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="H36" s="1">
-        <v>16.425000000000001</v>
+        <v>6.35</v>
       </c>
       <c r="I36" s="1">
-        <v>16.574999999999999</v>
+        <v>6.45</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1" t="s">
-        <v>302</v>
-      </c>
+      <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>146</v>
+        <v>216</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>147</v>
+        <v>217</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F37" s="6">
+        <v>218</v>
+      </c>
+      <c r="F37" s="5">
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="H37" s="1">
-        <v>9.8000000000000007</v>
+        <v>6.0724999999999998</v>
       </c>
       <c r="I37" s="1">
-        <v>10.1</v>
+        <v>6.25</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>251</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="F38" s="5">
+        <v>2</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="H38" s="1">
-        <v>3.8250000000000002</v>
+        <v>7.4</v>
       </c>
       <c r="I38" s="1">
-        <v>3.9249999999999998</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>283</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F39" s="6">
+        <v>102</v>
+      </c>
+      <c r="F39" s="5">
         <v>2</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="H39" s="1">
-        <v>5</v>
+        <v>19.45</v>
       </c>
       <c r="I39" s="1">
-        <v>5.2</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>318</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>257</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="F40" s="5">
+        <v>2</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="H40" s="1">
-        <v>11.9</v>
+        <v>4.3</v>
       </c>
       <c r="I40" s="1">
-        <v>12.2</v>
+        <v>4.45</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="L40" s="1"/>
+        <v>337</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" s="6">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="F41" s="5">
+        <v>2</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="H41" s="1">
-        <v>13.725</v>
+        <v>4.25</v>
       </c>
       <c r="I41" s="1">
-        <v>13.85</v>
+        <v>4.45</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>317</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>288</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="6">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="F42" s="5">
+        <v>2</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H42" s="7">
-        <v>6.05</v>
-      </c>
-      <c r="I42" s="7">
-        <v>6.25</v>
+        <v>322</v>
+      </c>
+      <c r="H42" s="1">
+        <v>11.05</v>
+      </c>
+      <c r="I42" s="1">
+        <v>11.25</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>321</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>59</v>
+        <v>183</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>60</v>
+        <v>184</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F43" s="6">
-        <v>1</v>
+        <v>185</v>
+      </c>
+      <c r="F43" s="5">
+        <v>2</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>292</v>
+        <v>335</v>
       </c>
       <c r="H43" s="1">
-        <v>19.3</v>
+        <v>17.149999999999999</v>
       </c>
       <c r="I43" s="1">
-        <v>19.600000000000001</v>
+        <v>17.45</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F44" s="6">
-        <v>1</v>
+        <v>215</v>
+      </c>
+      <c r="F44" s="5">
+        <v>2</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="H44" s="1">
-        <v>19.399999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="I44" s="1">
-        <v>19.7</v>
+        <v>7.55</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>252</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>152</v>
+        <v>221</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1</v>
+        <v>222</v>
+      </c>
+      <c r="F45" s="5">
+        <v>2</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="H45" s="1">
-        <v>8.0500000000000007</v>
+        <v>5.15</v>
       </c>
       <c r="I45" s="1">
-        <v>8.35</v>
+        <v>5.3</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>343</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F46" s="6">
-        <v>1</v>
+        <v>225</v>
+      </c>
+      <c r="F46" s="5">
+        <v>2</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>348</v>
+        <v>295</v>
       </c>
       <c r="H46" s="1">
-        <v>17.8</v>
+        <v>12.7</v>
       </c>
       <c r="I46" s="1">
-        <v>18</v>
+        <v>12.875</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>122</v>
+        <v>229</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="6">
+        <v>227</v>
+      </c>
+      <c r="F47" s="5">
         <v>2</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>335</v>
+        <v>271</v>
       </c>
       <c r="H47" s="1">
-        <v>12.85</v>
+        <v>7.2</v>
       </c>
       <c r="I47" s="1">
-        <v>13.025</v>
+        <v>7.4</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="6">
-        <v>1</v>
+        <v>231</v>
+      </c>
+      <c r="F48" s="5">
+        <v>2</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
       <c r="H48" s="1">
-        <v>7.9749999999999996</v>
+        <v>16.425000000000001</v>
       </c>
       <c r="I48" s="1">
-        <v>8.15</v>
+        <v>16.574999999999999</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>310</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="K48" s="1"/>
       <c r="L48" s="1" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" s="6">
-        <v>2</v>
+        <v>200</v>
+      </c>
+      <c r="F49" s="5">
+        <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="H49" s="1">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="I49" s="1">
-        <v>6.6</v>
+        <v>6.55</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="L49" s="1"/>
+        <v>337</v>
+      </c>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="G50" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="H50" s="1">
-        <v>4.3</v>
+        <v>20</v>
       </c>
       <c r="I50" s="1">
-        <v>4.9000000000000004</v>
+        <v>20.2</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="L50" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>121</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>199</v>
+        <v>122</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F51" s="8">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>268</v>
+        <v>323</v>
       </c>
       <c r="H51" s="1">
-        <v>6.4</v>
+        <v>12.85</v>
       </c>
       <c r="I51" s="1">
-        <v>6.55</v>
+        <v>13.025</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="K51" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="L51" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F52" s="6">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H52" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I52" s="1">
-        <v>20.2</v>
+        <v>5.2</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="L52" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F53" s="6">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="H53" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="I53" s="1">
-        <v>7.5</v>
+        <v>194</v>
+      </c>
+      <c r="H53" s="9">
+        <v>6.05</v>
+      </c>
+      <c r="I53" s="9">
+        <v>6.25</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="K53" s="1"/>
       <c r="L53" s="1" t="s">
-        <v>246</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>220</v>
+        <v>9</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H54" s="1">
-        <v>5.75</v>
-      </c>
-      <c r="I54" s="1">
-        <v>6.0250000000000004</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="K54" s="1"/>
       <c r="L54" s="1" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>202</v>
+        <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>200</v>
+        <v>12</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H55" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="I55" s="1">
-        <v>6.45</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>210</v>
+        <v>13</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="H56" s="1">
-        <v>6.5750000000000002</v>
-      </c>
-      <c r="I56" s="1">
-        <v>6.7</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1" t="s">
-        <v>307</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>226</v>
+        <v>29</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>214</v>
+        <v>30</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H57" s="1">
-        <v>7.05</v>
-      </c>
-      <c r="I57" s="1">
-        <v>7.25</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K58" s="1"/>
-      <c r="L58" s="1" t="s">
-        <v>275</v>
-      </c>
+      <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K59" s="1"/>
       <c r="L59" s="1" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
+      <c r="L62" s="1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K63" s="1"/>
-      <c r="L63" s="1" t="s">
-        <v>287</v>
-      </c>
+      <c r="L63" s="1"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1" t="s">
-        <v>258</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>68</v>
+        <v>327</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K65" s="1"/>
-      <c r="L65" s="1" t="s">
-        <v>319</v>
-      </c>
+      <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="L66" s="1" t="s">
-        <v>320</v>
-      </c>
+      <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
+      <c r="L67" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K68" s="1"/>
       <c r="L68" s="1" t="s">
-        <v>326</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>339</v>
+        <v>159</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
+      <c r="L69" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
+      <c r="L70" s="1" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K71" s="1"/>
-      <c r="L71" s="1" t="s">
-        <v>342</v>
-      </c>
+      <c r="L71" s="1"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1" t="s">
@@ -4025,276 +3994,302 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1" t="s">
-        <v>191</v>
+        <v>305</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1" t="s">
-        <v>346</v>
+        <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
+      <c r="L75" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1" t="s">
-        <v>191</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
+        <v>292</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H78" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="I78" s="1">
+        <v>6.0250000000000004</v>
+      </c>
       <c r="J78" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K78" s="1"/>
       <c r="L78" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H79" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="I79" s="1">
+        <v>6.45</v>
+      </c>
       <c r="J79" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K79" s="1"/>
       <c r="L79" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" s="1">
+        <v>6.5750000000000002</v>
+      </c>
+      <c r="I80" s="1">
+        <v>6.7</v>
+      </c>
       <c r="J80" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F81" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
+      <c r="H81" s="1">
+        <v>7.05</v>
+      </c>
+      <c r="I81" s="1">
+        <v>7.25</v>
+      </c>
       <c r="J81" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L81" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L81">
-      <sortCondition ref="J1:J81"/>
+      <sortCondition descending="1" ref="J1:J81"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
began working on pulling in final files
</commit_message>
<xml_diff>
--- a/metadata_files/variant_validation.xlsx
+++ b/metadata_files/variant_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdp2019/Desktop/thyroid-exposomics-2025/metadata_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33B4DB0-A1DC-BF4D-A259-266A80CF3624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC49319-5BEC-6F48-BF76-0F22770E6577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="19140" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="360">
   <si>
     <t>order</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>Consider making level 2 but move to smaller x window</t>
+  </si>
+  <si>
+    <t>F1_S1_CP2487, F1_S2_CP2487, F2_S1_CP2487, F2_S2_CP2487, F3_S1_CP2487, F3_S2_CP2487, F4_S1_CP2487, F4_S2_CP2487, F5_S1_CP2487, F5_S2_CP2487, F6_S1_CP2487, F6_S2_CP2487</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1197,10 +1200,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1539,7 +1541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1552,7 @@
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="7.1640625" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
@@ -1596,7 +1598,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -1632,7 +1634,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>41</v>
       </c>
@@ -1651,7 +1653,9 @@
       <c r="F3" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="H3" s="1">
         <v>4.3</v>
       </c>
@@ -1666,7 +1670,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42</v>
       </c>
@@ -1704,7 +1708,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>59</v>
       </c>
@@ -1742,7 +1746,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>28</v>
       </c>
@@ -1778,7 +1782,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>19</v>
       </c>
@@ -1794,7 +1798,7 @@
       <c r="E7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1814,7 +1818,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>51</v>
       </c>
@@ -1850,7 +1854,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1866,7 +1870,7 @@
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="5">
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1878,7 +1882,7 @@
       <c r="I9" s="1">
         <v>3.9249999999999998</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="1" t="s">
         <v>354</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1888,7 +1892,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>49</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>56</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1976,7 +1980,7 @@
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1998,7 +2002,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>15</v>
       </c>
@@ -2014,7 +2018,7 @@
       <c r="E13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2034,7 +2038,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -2142,7 +2146,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>20</v>
       </c>
@@ -2212,7 +2216,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>21</v>
       </c>
@@ -2246,7 +2250,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>24</v>
       </c>
@@ -2280,7 +2284,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>26</v>
       </c>
@@ -2314,7 +2318,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>27</v>
       </c>
@@ -2348,7 +2352,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>29</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>30</v>
       </c>
@@ -2420,7 +2424,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>34</v>
       </c>
@@ -2454,7 +2458,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>35</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>36</v>
       </c>
@@ -2526,7 +2530,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45</v>
       </c>
@@ -2594,7 +2598,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>47</v>
       </c>
@@ -2628,7 +2632,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>48</v>
       </c>
@@ -2662,7 +2666,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>54</v>
       </c>
@@ -2696,7 +2700,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>55</v>
       </c>
@@ -2730,7 +2734,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>58</v>
       </c>
@@ -2764,7 +2768,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>60</v>
       </c>
@@ -2798,7 +2802,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>65</v>
       </c>
@@ -2832,7 +2836,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>72</v>
       </c>
@@ -2866,7 +2870,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>8</v>
       </c>
@@ -2902,7 +2906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>33</v>
       </c>
@@ -2938,7 +2942,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -3010,7 +3014,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -3044,7 +3048,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>62</v>
       </c>
@@ -3078,7 +3082,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>71</v>
       </c>
@@ -3112,7 +3116,7 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>74</v>
       </c>
@@ -3146,7 +3150,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>75</v>
       </c>
@@ -3180,7 +3184,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>77</v>
       </c>
@@ -3214,7 +3218,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>78</v>
       </c>
@@ -3250,7 +3254,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>64</v>
       </c>
@@ -3286,7 +3290,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>14</v>
       </c>
@@ -3302,7 +3306,7 @@
       <c r="E50" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="5" t="s">
         <v>277</v>
       </c>
       <c r="G50" s="1" t="s">
@@ -3322,7 +3326,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>40</v>
       </c>
@@ -3338,7 +3342,7 @@
       <c r="E51" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="5" t="s">
         <v>277</v>
       </c>
       <c r="G51" s="1" t="s">
@@ -3360,7 +3364,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>16</v>
       </c>
@@ -3376,7 +3380,7 @@
       <c r="E52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="5" t="s">
         <v>277</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -3396,7 +3400,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>25</v>
       </c>
@@ -3412,16 +3416,16 @@
       <c r="E53" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="5" t="s">
         <v>277</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="1">
         <v>6.05</v>
       </c>
-      <c r="I53" s="9">
+      <c r="I53" s="1">
         <v>6.25</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -3432,7 +3436,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2</v>
       </c>
@@ -3462,7 +3466,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -3492,7 +3496,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>4</v>
       </c>
@@ -3522,7 +3526,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>9</v>
       </c>
@@ -3552,7 +3556,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>11</v>
       </c>
@@ -3580,7 +3584,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>12</v>
       </c>
@@ -3610,7 +3614,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>18</v>
       </c>
@@ -3640,7 +3644,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>22</v>
       </c>
@@ -3670,7 +3674,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>23</v>
       </c>
@@ -3700,7 +3704,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>31</v>
       </c>
@@ -3728,7 +3732,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>32</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44</v>
       </c>
@@ -3786,7 +3790,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>46</v>
       </c>
@@ -3814,7 +3818,7 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>50</v>
       </c>
@@ -3844,7 +3848,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>52</v>
       </c>
@@ -3874,7 +3878,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>53</v>
       </c>
@@ -3904,7 +3908,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>57</v>
       </c>
@@ -3934,7 +3938,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>61</v>
       </c>
@@ -3962,7 +3966,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>63</v>
       </c>
@@ -3992,7 +3996,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>67</v>
       </c>
@@ -4022,7 +4026,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>79</v>
       </c>
@@ -4052,7 +4056,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>68</v>
       </c>
@@ -4082,7 +4086,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>69</v>
       </c>
@@ -4112,7 +4116,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>80</v>
       </c>
@@ -4142,7 +4146,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>73</v>
       </c>
@@ -4178,7 +4182,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>66</v>
       </c>
@@ -4214,7 +4218,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>70</v>
       </c>
@@ -4250,7 +4254,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
directory in onedrive changed to curated
</commit_message>
<xml_diff>
--- a/metadata_files/variant_validation.xlsx
+++ b/metadata_files/variant_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B6F2F8-C7BE-404E-AEC0-D3EA74A83D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8D13BA-4758-1C45-9344-26358E3E9103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="19140" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="33880" windowHeight="19140" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
worked on plot formation
</commit_message>
<xml_diff>
--- a/metadata_files/variant_validation.xlsx
+++ b/metadata_files/variant_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoshsMacbook2015/Desktop/thyroid-exposomics-2025/metadata_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8D13BA-4758-1C45-9344-26358E3E9103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE325238-542A-1749-915C-E5F16EB6712D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="33880" windowHeight="19140" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
+    <workbookView xWindow="0" yWindow="1640" windowWidth="38000" windowHeight="19020" xr2:uid="{46DE10B9-3B48-7244-99C1-85EF65A7D9FA}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="361">
   <si>
     <t>order</t>
   </si>
@@ -794,9 +794,6 @@
     <t>F2_S1_CP2382</t>
   </si>
   <si>
-    <t xml:space="preserve">Has 2 Peaks in Standard and Sample, but the quantifying one is incredibly low abundance </t>
-  </si>
-  <si>
     <t>window ranges are different</t>
   </si>
   <si>
@@ -1073,9 +1070,6 @@
     <t>initial huge peak way to left but not annotated one</t>
   </si>
   <si>
-    <t>final (check frag)</t>
-  </si>
-  <si>
     <t>modify</t>
   </si>
   <si>
@@ -1119,6 +1113,15 @@
   </si>
   <si>
     <t>F1_S1_CP2487, F1_S2_CP2487, F2_S1_CP2487, F2_S2_CP2487, F3_S1_CP2487, F3_S2_CP2487, F4_S1_CP2487, F4_S2_CP2487, F5_S1_CP2487, F5_S2_CP2487, F6_S1_CP2487, F6_S2_CP2487</t>
+  </si>
+  <si>
+    <t>final- failed</t>
+  </si>
+  <si>
+    <t>quant fragment visible and very tiny but still coelutes, pass</t>
+  </si>
+  <si>
+    <t>x axis zoomed in</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1202,6 +1205,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1540,19 +1547,19 @@
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="7.1640625" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
@@ -1577,22 +1584,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>236</v>
@@ -1600,2700 +1607,2704 @@
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="6">
-        <v>2</v>
+        <v>220</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>291</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="H2" s="1">
-        <v>6.3</v>
+        <v>5.75</v>
       </c>
       <c r="I2" s="1">
-        <v>6.6</v>
+        <v>6.0250000000000004</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="L2" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>237</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>359</v>
+        <v>200</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="H3" s="1">
-        <v>4.3</v>
+        <v>6.35</v>
       </c>
       <c r="I3" s="1">
-        <v>4.9000000000000004</v>
+        <v>6.45</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="L3" s="1"/>
+        <v>351</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
+        <v>212</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H4" s="1">
-        <v>7.3</v>
+        <v>6.5750000000000002</v>
       </c>
       <c r="I4" s="1">
-        <v>7.5</v>
+        <v>6.7</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>358</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>246</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
+        <v>227</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="H5" s="1">
-        <v>17.8</v>
+        <v>7.05</v>
       </c>
       <c r="I5" s="1">
-        <v>18</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>7.25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H6" s="1">
-        <v>11.9</v>
-      </c>
-      <c r="I6" s="1">
-        <v>12.2</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="L6" s="1"/>
+        <v>205</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>204</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="H7" s="1">
-        <v>19.3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L7" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>152</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>153</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H8" s="1">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8.35</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="L8" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3.8250000000000002</v>
-      </c>
-      <c r="I9" s="1">
-        <v>3.9249999999999998</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>346</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>343</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H10" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="I10" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>344</v>
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>166</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>167</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="H11" s="1">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="I11" s="1">
-        <v>19.7</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>344</v>
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>252</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H12" s="1">
-        <v>7.9749999999999996</v>
-      </c>
-      <c r="I12" s="1">
-        <v>8.15</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>272</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H13" s="1">
-        <v>13.725</v>
-      </c>
-      <c r="I13" s="1">
-        <v>13.85</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H14" s="1">
-        <v>7.85</v>
-      </c>
-      <c r="I14" s="1">
-        <v>7.9249999999999998</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="5">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H15" s="1">
-        <v>13.25</v>
-      </c>
-      <c r="I15" s="1">
-        <v>13.45</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="5">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="H16" s="1">
-        <v>13.425000000000001</v>
-      </c>
-      <c r="I16" s="1">
-        <v>13.574999999999999</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="5">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H17" s="1">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1">
-        <v>3.4</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="5">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H18" s="1">
-        <v>6.35</v>
-      </c>
-      <c r="I18" s="1">
-        <v>6.5</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>326</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H19" s="1">
-        <v>6.375</v>
-      </c>
-      <c r="I19" s="1">
-        <v>6.5</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="1">
-        <v>9.0500000000000007</v>
-      </c>
-      <c r="I20" s="1">
-        <v>9.2249999999999996</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H21" s="1">
-        <v>9.5749999999999993</v>
-      </c>
-      <c r="I21" s="1">
-        <v>9.7750000000000004</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="5">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="H22" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="I22" s="1">
-        <v>3.95</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>89</v>
+        <v>159</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="H23" s="1">
-        <v>9.4</v>
-      </c>
-      <c r="I23" s="1">
-        <v>9.65</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>312</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="H24" s="1">
-        <v>11.2</v>
-      </c>
-      <c r="I24" s="1">
-        <v>11.3575</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1" t="s">
-        <v>259</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>103</v>
+        <v>180</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>104</v>
+        <v>181</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H25" s="1">
-        <v>22.3</v>
-      </c>
-      <c r="I25" s="1">
-        <v>22.45</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>187</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="5">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="H26" s="1">
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="I26" s="1">
-        <v>9.65</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>109</v>
+        <v>206</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>110</v>
+        <v>207</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H27" s="1">
-        <v>9.35</v>
-      </c>
-      <c r="I27" s="1">
-        <v>9.5500000000000007</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
-        <v>244</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" s="5">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="I28" s="1">
-        <v>2.5</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>234</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F29" s="5">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H29" s="1">
-        <v>8.0250000000000004</v>
-      </c>
-      <c r="I29" s="1">
-        <v>8.25</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="L29" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>141</v>
+        <v>237</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>142</v>
+        <v>200</v>
       </c>
       <c r="F30" s="5">
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>328</v>
+        <v>266</v>
       </c>
       <c r="H30" s="1">
-        <v>18</v>
+        <v>6.35</v>
       </c>
       <c r="I30" s="1">
-        <v>18.149999999999999</v>
+        <v>6.45</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>143</v>
+        <v>216</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>144</v>
+        <v>217</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>218</v>
       </c>
       <c r="F31" s="5">
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
       <c r="H31" s="1">
-        <v>9.8000000000000007</v>
+        <v>6.0724999999999998</v>
       </c>
       <c r="I31" s="1">
-        <v>10.102499999999999</v>
+        <v>6.25</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="F32" s="5">
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H32" s="1">
-        <v>7.7</v>
+        <v>6.4</v>
       </c>
       <c r="I32" s="1">
-        <v>7.875</v>
+        <v>6.55</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="L32" s="1" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>165</v>
+        <v>49</v>
       </c>
       <c r="F33" s="5">
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>330</v>
+        <v>285</v>
       </c>
       <c r="H33" s="1">
-        <v>6.6</v>
+        <v>13.725</v>
       </c>
       <c r="I33" s="1">
-        <v>6.75</v>
+        <v>13.85</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="L33" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>172</v>
+        <v>22</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>173</v>
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>174</v>
+        <v>24</v>
       </c>
       <c r="F34" s="5">
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>332</v>
+        <v>252</v>
       </c>
       <c r="H34" s="1">
-        <v>4.9000000000000004</v>
+        <v>7.85</v>
       </c>
       <c r="I34" s="1">
-        <v>5.05</v>
+        <v>7.9249999999999998</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>179</v>
+        <v>34</v>
       </c>
       <c r="F35" s="5">
         <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H35" s="1">
+        <v>13.25</v>
+      </c>
+      <c r="I35" s="1">
+        <v>13.45</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="H35" s="1">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I35" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="L35" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>201</v>
+        <v>41</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>237</v>
+        <v>42</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>200</v>
+        <v>43</v>
       </c>
       <c r="F36" s="5">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
       <c r="H36" s="1">
-        <v>6.35</v>
+        <v>13.425000000000001</v>
       </c>
       <c r="I36" s="1">
-        <v>6.45</v>
+        <v>13.574999999999999</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
+      <c r="L36" s="1" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>216</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>218</v>
+        <v>55</v>
       </c>
       <c r="F37" s="5">
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H37" s="1">
-        <v>6.0724999999999998</v>
+        <v>3</v>
       </c>
       <c r="I37" s="1">
-        <v>6.25</v>
+        <v>3.4</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="L37" s="1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F38" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>254</v>
+        <v>192</v>
       </c>
       <c r="H38" s="1">
-        <v>7.4</v>
+        <v>6.35</v>
       </c>
       <c r="I38" s="1">
-        <v>7.5250000000000004</v>
+        <v>6.5</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K38" s="1"/>
-      <c r="L38" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="F39" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="H39" s="1">
-        <v>19.45</v>
+        <v>6.375</v>
       </c>
       <c r="I39" s="1">
-        <v>19.600000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K39" s="1"/>
-      <c r="L39" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="F40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>319</v>
+        <v>193</v>
       </c>
       <c r="H40" s="1">
-        <v>4.3</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="I40" s="1">
-        <v>4.45</v>
+        <v>9.2249999999999996</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
-        <v>320</v>
-      </c>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="F41" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>321</v>
+        <v>195</v>
       </c>
       <c r="H41" s="1">
-        <v>4.25</v>
+        <v>9.5749999999999993</v>
       </c>
       <c r="I41" s="1">
-        <v>4.45</v>
+        <v>9.7750000000000004</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="F42" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>322</v>
+        <v>196</v>
       </c>
       <c r="H42" s="1">
-        <v>11.05</v>
+        <v>3.8</v>
       </c>
       <c r="I42" s="1">
-        <v>11.25</v>
+        <v>3.95</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>184</v>
+        <v>89</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="F43" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="H43" s="1">
-        <v>17.149999999999999</v>
+        <v>9.4</v>
       </c>
       <c r="I43" s="1">
-        <v>17.45</v>
+        <v>9.65</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+      <c r="L43" s="1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>214</v>
+        <v>92</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>215</v>
+        <v>93</v>
       </c>
       <c r="F44" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="H44" s="1">
-        <v>7.4</v>
+        <v>11.2</v>
       </c>
       <c r="I44" s="1">
-        <v>7.55</v>
+        <v>11.3575</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="L44" s="1" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>221</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>222</v>
+        <v>105</v>
       </c>
       <c r="F45" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="H45" s="1">
-        <v>5.15</v>
+        <v>22.3</v>
       </c>
       <c r="I45" s="1">
-        <v>5.3</v>
+        <v>22.45</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>223</v>
+        <v>106</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>224</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>225</v>
+        <v>108</v>
       </c>
       <c r="F46" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>295</v>
+        <v>242</v>
       </c>
       <c r="H46" s="1">
-        <v>12.7</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="I46" s="1">
-        <v>12.875</v>
+        <v>9.65</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="L46" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>228</v>
+        <v>109</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>229</v>
+        <v>110</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>227</v>
+        <v>111</v>
       </c>
       <c r="F47" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>271</v>
+        <v>315</v>
       </c>
       <c r="H47" s="1">
-        <v>7.2</v>
+        <v>9.35</v>
       </c>
       <c r="I47" s="1">
-        <v>7.4</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="L47" s="1" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="F48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>299</v>
+        <v>247</v>
       </c>
       <c r="H48" s="1">
-        <v>16.425000000000001</v>
+        <v>2.25</v>
       </c>
       <c r="I48" s="1">
-        <v>16.574999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="L48" s="1" t="s">
-        <v>298</v>
-      </c>
+      <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="F49" s="5">
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="H49" s="1">
-        <v>6.4</v>
+        <v>8.0250000000000004</v>
       </c>
       <c r="I49" s="1">
-        <v>6.55</v>
+        <v>8.25</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K49" s="1"/>
-      <c r="L49" s="1" t="s">
-        <v>342</v>
-      </c>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>277</v>
+        <v>142</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>255</v>
+        <v>327</v>
       </c>
       <c r="H50" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I50" s="1">
-        <v>20.2</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K50" s="1"/>
-      <c r="L50" s="1" t="s">
-        <v>357</v>
-      </c>
+      <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>277</v>
+        <v>145</v>
+      </c>
+      <c r="F51" s="5">
+        <v>1</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>323</v>
+        <v>249</v>
       </c>
       <c r="H51" s="1">
-        <v>12.85</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I51" s="1">
-        <v>13.025</v>
+        <v>10.102499999999999</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>355</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>277</v>
+        <v>154</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="H52" s="1">
-        <v>5</v>
+        <v>7.7</v>
       </c>
       <c r="I52" s="1">
-        <v>5.2</v>
+        <v>7.875</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K52" s="1"/>
-      <c r="L52" s="1" t="s">
-        <v>347</v>
-      </c>
+      <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>277</v>
+        <v>165</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>194</v>
+        <v>329</v>
       </c>
       <c r="H53" s="1">
-        <v>6.05</v>
+        <v>6.6</v>
       </c>
       <c r="I53" s="1">
-        <v>6.25</v>
+        <v>6.75</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K53" s="1"/>
-      <c r="L53" s="1" t="s">
-        <v>350</v>
-      </c>
+      <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H54" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I54" s="1">
+        <v>5.05</v>
+      </c>
       <c r="J54" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K54" s="1"/>
-      <c r="L54" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>10</v>
+        <v>177</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="F55" s="5">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H55" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I55" s="1">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="J55" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="L55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="F56" s="5">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H56" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="I56" s="1">
+        <v>7.55</v>
+      </c>
       <c r="J56" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="1" t="s">
-        <v>278</v>
-      </c>
+      <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>29</v>
+        <v>221</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>30</v>
+        <v>211</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
+        <v>222</v>
+      </c>
+      <c r="F57" s="5">
+        <v>2</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H57" s="1">
+        <v>5.15</v>
+      </c>
+      <c r="I57" s="1">
+        <v>5.3</v>
+      </c>
       <c r="J57" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="1" t="s">
-        <v>307</v>
-      </c>
+      <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+        <v>225</v>
+      </c>
+      <c r="F58" s="5">
+        <v>2</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H58" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="I58" s="1">
+        <v>12.875</v>
+      </c>
       <c r="J58" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>38</v>
+        <v>228</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>39</v>
+        <v>229</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="F59" s="5">
+        <v>2</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H59" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="I59" s="1">
+        <v>7.4</v>
+      </c>
       <c r="J59" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K59" s="1"/>
-      <c r="L59" s="1" t="s">
-        <v>284</v>
-      </c>
+      <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>56</v>
+        <v>230</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>57</v>
+        <v>207</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="F60" s="5">
+        <v>2</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H60" s="1">
+        <v>16.425000000000001</v>
+      </c>
+      <c r="I60" s="1">
+        <v>16.574999999999999</v>
+      </c>
       <c r="J60" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1" t="s">
-        <v>257</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="F61" s="5">
+        <v>2</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H61" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="I61" s="1">
+        <v>7.5250000000000004</v>
+      </c>
       <c r="J61" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="1" t="s">
-        <v>310</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="F62" s="5">
+        <v>2</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H62" s="1">
+        <v>19.45</v>
+      </c>
+      <c r="I62" s="1">
+        <v>19.600000000000001</v>
+      </c>
       <c r="J62" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1" t="s">
-        <v>311</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="F63" s="5">
+        <v>2</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H63" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="I63" s="1">
+        <v>4.45</v>
+      </c>
       <c r="J63" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
+      <c r="L63" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="64" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="F64" s="5">
+        <v>2</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H64" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="I64" s="1">
+        <v>4.45</v>
+      </c>
       <c r="J64" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1" t="s">
-        <v>315</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>327</v>
+        <v>119</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="F65" s="5">
+        <v>2</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H65" s="1">
+        <v>11.05</v>
+      </c>
+      <c r="I65" s="1">
+        <v>11.25</v>
+      </c>
       <c r="J65" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
     <row r="66" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
+        <v>185</v>
+      </c>
+      <c r="F66" s="5">
+        <v>2</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H66" s="1">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="I66" s="1">
+        <v>17.45</v>
+      </c>
       <c r="J66" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K67" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="F67" s="10">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H67" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I67" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="J67" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="L67" s="1" t="s">
-        <v>329</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K68" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="F68" s="10">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H68" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I68" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="J68" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="L68" s="1" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>158</v>
+        <v>44</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>160</v>
+        <v>46</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H69" s="1">
+        <v>20</v>
+      </c>
+      <c r="I69" s="1">
+        <v>20.2</v>
+      </c>
       <c r="J69" s="1" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1" t="s">
-        <v>191</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H70" s="1">
+        <v>12.85</v>
+      </c>
+      <c r="I70" s="1">
+        <v>13.025</v>
+      </c>
       <c r="J70" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K70" s="1"/>
+        <v>358</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="L70" s="1" t="s">
-        <v>331</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>182</v>
+        <v>52</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H71" s="1">
+        <v>5</v>
+      </c>
+      <c r="I71" s="1">
+        <v>5.2</v>
+      </c>
       <c r="J71" s="1" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
+      <c r="L71" s="1" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="72" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>186</v>
+        <v>76</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>188</v>
+        <v>78</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H72" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="I72" s="1">
+        <v>6.25</v>
+      </c>
       <c r="J72" s="1" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1" t="s">
-        <v>191</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>203</v>
+        <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>204</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F73" s="5">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H73" s="1">
+        <v>7.9749999999999996</v>
+      </c>
+      <c r="I73" s="1">
+        <v>8.15</v>
+      </c>
       <c r="J73" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K73" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="L73" s="1" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>232</v>
+        <v>16</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="F74" s="5">
+        <v>2</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H74" s="1">
+        <v>3.8250000000000002</v>
+      </c>
+      <c r="I74" s="1">
+        <v>3.9249999999999998</v>
+      </c>
       <c r="J74" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K74" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="L74" s="1" t="s">
-        <v>301</v>
+        <v>342</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K75" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="F75" s="6">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H75" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="I75" s="1">
+        <v>18</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="L75" s="1" t="s">
-        <v>300</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>209</v>
+        <v>85</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1" t="s">
-        <v>304</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F76" s="6">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H76" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="I76" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="L76" s="1"/>
     </row>
     <row r="77" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>234</v>
+        <v>59</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>199</v>
+        <v>60</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1" t="s">
-        <v>302</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F77" s="5">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H77" s="1">
+        <v>19.3</v>
+      </c>
+      <c r="I77" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="L77" s="1"/>
     </row>
     <row r="78" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>219</v>
+        <v>152</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>292</v>
+        <v>154</v>
+      </c>
+      <c r="F78" s="6">
+        <v>1</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="H78" s="1">
-        <v>5.75</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="I78" s="1">
-        <v>6.0250000000000004</v>
-      </c>
-      <c r="J78" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>8.35</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>202</v>
+        <v>127</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>294</v>
+        <v>129</v>
+      </c>
+      <c r="F79" s="6">
+        <v>1</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="H79" s="1">
-        <v>6.35</v>
+        <v>7.3</v>
       </c>
       <c r="I79" s="1">
-        <v>6.45</v>
+        <v>7.5</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="K79" s="1"/>
+        <v>339</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="L79" s="1" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>210</v>
+        <v>19</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>211</v>
+        <v>20</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>294</v>
+        <v>21</v>
+      </c>
+      <c r="F80" s="6">
+        <v>2</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="H80" s="1">
-        <v>6.5750000000000002</v>
+        <v>6.3</v>
       </c>
       <c r="I80" s="1">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L80" s="1"/>
     </row>
     <row r="81" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>226</v>
+        <v>124</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>297</v>
+        <v>126</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>357</v>
       </c>
       <c r="H81" s="1">
-        <v>7.05</v>
+        <v>4.3</v>
       </c>
       <c r="I81" s="1">
-        <v>7.25</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1" t="s">
-        <v>296</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="L81" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L81" xr:uid="{D6206EC4-7047-AB43-8209-3740D839E512}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L81">
-      <sortCondition descending="1" ref="J1:J81"/>
+      <sortCondition ref="J1:J81"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>